<commit_message>
added code for generating Supp Fig 19
</commit_message>
<xml_diff>
--- a/Supplementary_Tables_1_2_3.xlsx
+++ b/Supplementary_Tables_1_2_3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="260">
   <si>
     <t>genomic feature name</t>
   </si>
@@ -42,219 +42,234 @@
     <t>ECK120000885</t>
   </si>
   <si>
+    <t>ECK120010201</t>
+  </si>
+  <si>
     <t>ECK120000886</t>
   </si>
   <si>
-    <t>ECK120010201</t>
-  </si>
-  <si>
     <t>ECK125143560</t>
   </si>
   <si>
+    <t>ECK120010871</t>
+  </si>
+  <si>
+    <t>ECK120002891/ECK120002892</t>
+  </si>
+  <si>
     <t>ECK125143900</t>
   </si>
   <si>
+    <t>ECK120033617</t>
+  </si>
+  <si>
     <t>ECK120001548/ECK120002618</t>
   </si>
   <si>
     <t>ECK120013464</t>
   </si>
   <si>
-    <t>ECK120010871</t>
-  </si>
-  <si>
-    <t>ECK120033617</t>
-  </si>
-  <si>
     <t>ECK120010783</t>
   </si>
   <si>
+    <t>ECK120001091</t>
+  </si>
+  <si>
+    <t>ECK120000838</t>
+  </si>
+  <si>
     <t>ECK125144631</t>
   </si>
   <si>
-    <t>ECK120000838</t>
-  </si>
-  <si>
-    <t>ECK120001091</t>
-  </si>
-  <si>
     <t>ECK120000583</t>
   </si>
   <si>
-    <t>ECK120002891/ECK120002892</t>
+    <t>ECK120002403/ECK120000662</t>
+  </si>
+  <si>
+    <t>ECK120001349/ECK120004144</t>
+  </si>
+  <si>
+    <t>ECK120000276</t>
+  </si>
+  <si>
+    <t>ECK120002218</t>
+  </si>
+  <si>
+    <t>ECK120001833</t>
+  </si>
+  <si>
+    <t>ECK120033723</t>
+  </si>
+  <si>
+    <t>ECK120001029/ECK120030090</t>
   </si>
   <si>
     <t>ECK120000598/ECK120000296</t>
   </si>
   <si>
+    <t>ECK120002835</t>
+  </si>
+  <si>
     <t>ECK120001594</t>
   </si>
   <si>
-    <t>ECK120001029/ECK120030090</t>
-  </si>
-  <si>
-    <t>ECK120033723</t>
-  </si>
-  <si>
-    <t>ECK120001833</t>
-  </si>
-  <si>
-    <t>ECK120000276</t>
-  </si>
-  <si>
-    <t>ECK120002835</t>
-  </si>
-  <si>
-    <t>ECK120002403/ECK120000662</t>
+    <t>ECK120003553/ECK120003554</t>
+  </si>
+  <si>
+    <t>ECK120011926</t>
+  </si>
+  <si>
+    <t>ECK125136750</t>
+  </si>
+  <si>
+    <t>ECK120004249</t>
+  </si>
+  <si>
+    <t>ECK120003259</t>
+  </si>
+  <si>
+    <t>ECK120003261</t>
+  </si>
+  <si>
+    <t>ECK120003260</t>
+  </si>
+  <si>
+    <t>ECK125143996</t>
+  </si>
+  <si>
+    <t>ECK125143994</t>
+  </si>
+  <si>
+    <t>ECK125136881</t>
+  </si>
+  <si>
+    <t>ECK125136878</t>
+  </si>
+  <si>
+    <t>ECK125136882</t>
+  </si>
+  <si>
+    <t>ECK125136879</t>
+  </si>
+  <si>
+    <t>ECK120034219</t>
+  </si>
+  <si>
+    <t>ECK125136880</t>
+  </si>
+  <si>
+    <t>ECK120002520</t>
   </si>
   <si>
     <t>ECK120002341</t>
   </si>
   <si>
-    <t>ECK120003553/ECK120003554</t>
-  </si>
-  <si>
-    <t>ECK120002520</t>
-  </si>
-  <si>
-    <t>ECK125136882</t>
-  </si>
-  <si>
-    <t>ECK125136879</t>
-  </si>
-  <si>
-    <t>ECK125136881</t>
-  </si>
-  <si>
-    <t>ECK125136880</t>
-  </si>
-  <si>
-    <t>ECK120034219</t>
-  </si>
-  <si>
-    <t>ECK125136878</t>
-  </si>
-  <si>
-    <t>ECK125143994</t>
-  </si>
-  <si>
-    <t>ECK125143996</t>
-  </si>
-  <si>
-    <t>ECK120003260</t>
-  </si>
-  <si>
-    <t>ECK120003259</t>
-  </si>
-  <si>
-    <t>ECK120003261</t>
-  </si>
-  <si>
-    <t>ECK120004249</t>
-  </si>
-  <si>
-    <t>ECK125136750</t>
-  </si>
-  <si>
-    <t>ECK120001349/ECK120004144</t>
+    <t>ECK120000903</t>
+  </si>
+  <si>
+    <t>ECK120001254</t>
+  </si>
+  <si>
+    <t>ECK120004404/ECK120002319</t>
+  </si>
+  <si>
+    <t>ECK125137156</t>
+  </si>
+  <si>
+    <t>ECK120001976</t>
+  </si>
+  <si>
+    <t>ECK120001961</t>
+  </si>
+  <si>
+    <t>ECK125137284</t>
+  </si>
+  <si>
+    <t>ECK120000133</t>
+  </si>
+  <si>
+    <t>ECK120003634</t>
+  </si>
+  <si>
+    <t>ECK120000314</t>
+  </si>
+  <si>
+    <t>ECK120003439</t>
+  </si>
+  <si>
+    <t>ECK120002031/ECK120001303</t>
+  </si>
+  <si>
+    <t>ECK120003438</t>
+  </si>
+  <si>
+    <t>ECK120002238</t>
+  </si>
+  <si>
+    <t>ECK120001543</t>
+  </si>
+  <si>
+    <t>ECK120002998</t>
+  </si>
+  <si>
+    <t>ECK120002806</t>
+  </si>
+  <si>
+    <t>ECK120001044/ECK120003456</t>
+  </si>
+  <si>
+    <t>ECK120002230</t>
+  </si>
+  <si>
+    <t>ECK120003870</t>
+  </si>
+  <si>
+    <t>ECK120000620</t>
+  </si>
+  <si>
+    <t>ECK120000101</t>
+  </si>
+  <si>
+    <t>ECK120001784</t>
+  </si>
+  <si>
+    <t>ECK120001745</t>
+  </si>
+  <si>
+    <t>ECK120016925</t>
+  </si>
+  <si>
+    <t>ECK120011932</t>
+  </si>
+  <si>
+    <t>ECK120002346/ECK120002347</t>
+  </si>
+  <si>
+    <t>ECK120002200</t>
+  </si>
+  <si>
+    <t>ECK120002285/ECK120001647</t>
+  </si>
+  <si>
+    <t>ECK120010797</t>
+  </si>
+  <si>
+    <t>ECK120003833</t>
+  </si>
+  <si>
+    <t>ECK120000160</t>
+  </si>
+  <si>
+    <t>ECK125257016</t>
+  </si>
+  <si>
+    <t>ECK120003992/ECK120003993</t>
   </si>
   <si>
     <t>ECK120003274/ECK120003275</t>
   </si>
   <si>
-    <t>ECK120000903</t>
-  </si>
-  <si>
-    <t>ECK120011926</t>
-  </si>
-  <si>
-    <t>ECK120001044/ECK120003456</t>
-  </si>
-  <si>
-    <t>ECK120002998</t>
-  </si>
-  <si>
-    <t>ECK120001543</t>
-  </si>
-  <si>
-    <t>ECK120003438</t>
-  </si>
-  <si>
-    <t>ECK120003439</t>
-  </si>
-  <si>
-    <t>ECK125137156</t>
-  </si>
-  <si>
-    <t>ECK120000314</t>
-  </si>
-  <si>
-    <t>ECK120003634</t>
-  </si>
-  <si>
-    <t>ECK120000133</t>
-  </si>
-  <si>
-    <t>ECK125137284</t>
-  </si>
-  <si>
-    <t>ECK120001961</t>
-  </si>
-  <si>
-    <t>ECK120001976</t>
-  </si>
-  <si>
-    <t>ECK120002230</t>
-  </si>
-  <si>
-    <t>ECK120003870</t>
-  </si>
-  <si>
-    <t>ECK120000101</t>
-  </si>
-  <si>
-    <t>ECK120001784</t>
-  </si>
-  <si>
-    <t>ECK120001745</t>
-  </si>
-  <si>
-    <t>ECK120016925</t>
-  </si>
-  <si>
-    <t>ECK120011932</t>
-  </si>
-  <si>
-    <t>ECK120002346/ECK120002347</t>
-  </si>
-  <si>
-    <t>ECK120002200</t>
-  </si>
-  <si>
-    <t>ECK120002285/ECK120001647</t>
-  </si>
-  <si>
-    <t>ECK120010797</t>
-  </si>
-  <si>
-    <t>ECK120003833</t>
-  </si>
-  <si>
-    <t>ECK120000160</t>
-  </si>
-  <si>
-    <t>ECK125257016</t>
-  </si>
-  <si>
-    <t>ECK120003992/ECK120003993</t>
-  </si>
-  <si>
-    <t>ECK120002031/ECK120001303</t>
-  </si>
-  <si>
-    <t>ECK120004404/ECK120002319</t>
-  </si>
-  <si>
     <t>ECK120002259</t>
   </si>
   <si>
@@ -273,216 +288,231 @@
     <t>rpoB</t>
   </si>
   <si>
+    <t>hnsp</t>
+  </si>
+  <si>
     <t>rpoC</t>
   </si>
   <si>
-    <t>hnsp</t>
-  </si>
-  <si>
     <t>leuLABCD attenuator terminator</t>
   </si>
   <si>
+    <t>rpsMKD-rpoA-rplQ terminator</t>
+  </si>
+  <si>
+    <t>glxK/allE</t>
+  </si>
+  <si>
     <t>yceK attenuator terminator</t>
   </si>
   <si>
+    <t>yhdNp</t>
+  </si>
+  <si>
     <t>mstA/C0614</t>
   </si>
   <si>
     <t>glpFKX TFBS</t>
   </si>
   <si>
-    <t>rpsMKD-rpoA-rplQ terminator</t>
-  </si>
-  <si>
-    <t>yhdNp</t>
-  </si>
-  <si>
     <t>opgGH terminator</t>
   </si>
   <si>
+    <t>fimZ</t>
+  </si>
+  <si>
+    <t>rhsB</t>
+  </si>
+  <si>
     <t>metY-rimP-nusA-infB-rbfA-truB-rpsO-pnp attenuator terminator</t>
   </si>
   <si>
-    <t>rhsB</t>
-  </si>
-  <si>
-    <t>fimZ</t>
-  </si>
-  <si>
     <t>metL</t>
   </si>
   <si>
-    <t>glxK/allE</t>
+    <t>matP/ompA</t>
+  </si>
+  <si>
+    <t>glgS/yqiJ</t>
+  </si>
+  <si>
+    <t>fbaA</t>
+  </si>
+  <si>
+    <t>ettA</t>
+  </si>
+  <si>
+    <t>gldA</t>
+  </si>
+  <si>
+    <t>yfdXp</t>
+  </si>
+  <si>
+    <t>tyrB/yjbS</t>
   </si>
   <si>
     <t>mrcB/fhuA</t>
   </si>
   <si>
+    <t>yaiT</t>
+  </si>
+  <si>
     <t>yafD</t>
   </si>
   <si>
-    <t>tyrB/yjbS</t>
-  </si>
-  <si>
-    <t>yfdXp</t>
-  </si>
-  <si>
-    <t>gldA</t>
-  </si>
-  <si>
-    <t>fbaA</t>
-  </si>
-  <si>
-    <t>yaiT</t>
-  </si>
-  <si>
-    <t>matP/ompA</t>
+    <t>yeaD/yeaE</t>
+  </si>
+  <si>
+    <t>hns TFBS</t>
+  </si>
+  <si>
+    <t>yceQp6</t>
+  </si>
+  <si>
+    <t>gspE</t>
+  </si>
+  <si>
+    <t>pgrR</t>
+  </si>
+  <si>
+    <t>ynaI</t>
+  </si>
+  <si>
+    <t>mppA</t>
+  </si>
+  <si>
+    <t>insH-4 attenuator terminator</t>
+  </si>
+  <si>
+    <t>ynaI attenuator terminator</t>
+  </si>
+  <si>
+    <t>mppAp13</t>
+  </si>
+  <si>
+    <t>mppAp4</t>
+  </si>
+  <si>
+    <t>insHp7</t>
+  </si>
+  <si>
+    <t>mppAp5</t>
+  </si>
+  <si>
+    <t>ynaIp</t>
+  </si>
+  <si>
+    <t>mppAp9</t>
+  </si>
+  <si>
+    <t>rrlB</t>
   </si>
   <si>
     <t>gntK</t>
   </si>
   <si>
-    <t>yeaD/yeaE</t>
-  </si>
-  <si>
-    <t>rrlB</t>
-  </si>
-  <si>
-    <t>insHp7</t>
-  </si>
-  <si>
-    <t>mppAp5</t>
-  </si>
-  <si>
-    <t>mppAp13</t>
-  </si>
-  <si>
-    <t>mppAp9</t>
-  </si>
-  <si>
-    <t>ynaIp</t>
-  </si>
-  <si>
-    <t>mppAp4</t>
-  </si>
-  <si>
-    <t>ynaI attenuator terminator</t>
-  </si>
-  <si>
-    <t>insH-4 attenuator terminator</t>
-  </si>
-  <si>
-    <t>mppA</t>
-  </si>
-  <si>
-    <t>pgrR</t>
-  </si>
-  <si>
-    <t>ynaI</t>
-  </si>
-  <si>
-    <t>gspE</t>
-  </si>
-  <si>
-    <t>yceQp6</t>
-  </si>
-  <si>
-    <t>glgS/yqiJ</t>
+    <t>rpsM</t>
+  </si>
+  <si>
+    <t>mutL</t>
+  </si>
+  <si>
+    <t>yjhU/yjhF</t>
+  </si>
+  <si>
+    <t>flhCp3</t>
+  </si>
+  <si>
+    <t>napA</t>
+  </si>
+  <si>
+    <t>radD</t>
+  </si>
+  <si>
+    <t>rplYp3</t>
+  </si>
+  <si>
+    <t>cdd</t>
+  </si>
+  <si>
+    <t>yedP</t>
+  </si>
+  <si>
+    <t>flhD</t>
+  </si>
+  <si>
+    <t>clcB</t>
+  </si>
+  <si>
+    <t>uraA/upp</t>
+  </si>
+  <si>
+    <t>dmsD</t>
+  </si>
+  <si>
+    <t>intE</t>
+  </si>
+  <si>
+    <t>moaA</t>
+  </si>
+  <si>
+    <t>ybhD</t>
+  </si>
+  <si>
+    <t>yahI</t>
+  </si>
+  <si>
+    <t>uidA/uidR</t>
+  </si>
+  <si>
+    <t>menF</t>
+  </si>
+  <si>
+    <t>tmcA</t>
+  </si>
+  <si>
+    <t>mutY</t>
+  </si>
+  <si>
+    <t>atpH</t>
+  </si>
+  <si>
+    <t>yiiD</t>
+  </si>
+  <si>
+    <t>aidB</t>
+  </si>
+  <si>
+    <t>yjhW</t>
+  </si>
+  <si>
+    <t>mdaB/ygiN</t>
+  </si>
+  <si>
+    <t>yadK</t>
+  </si>
+  <si>
+    <t>tomB/acrB</t>
+  </si>
+  <si>
+    <t>ptsHI-crr terminator</t>
+  </si>
+  <si>
+    <t>pdxK</t>
+  </si>
+  <si>
+    <t>crp</t>
+  </si>
+  <si>
+    <t>carAB terminator</t>
+  </si>
+  <si>
+    <t>casD/casC</t>
   </si>
   <si>
     <t>ydaG/racR</t>
   </si>
   <si>
-    <t>rpsM</t>
-  </si>
-  <si>
-    <t>hns TFBS</t>
-  </si>
-  <si>
-    <t>uidA/uidR</t>
-  </si>
-  <si>
-    <t>ybhD</t>
-  </si>
-  <si>
-    <t>moaA</t>
-  </si>
-  <si>
-    <t>dmsD</t>
-  </si>
-  <si>
-    <t>clcB</t>
-  </si>
-  <si>
-    <t>flhCp3</t>
-  </si>
-  <si>
-    <t>flhD</t>
-  </si>
-  <si>
-    <t>yedP</t>
-  </si>
-  <si>
-    <t>cdd</t>
-  </si>
-  <si>
-    <t>rplYp3</t>
-  </si>
-  <si>
-    <t>radD</t>
-  </si>
-  <si>
-    <t>napA</t>
-  </si>
-  <si>
-    <t>menF</t>
-  </si>
-  <si>
-    <t>tmcA</t>
-  </si>
-  <si>
-    <t>atpH</t>
-  </si>
-  <si>
-    <t>yiiD</t>
-  </si>
-  <si>
-    <t>aidB</t>
-  </si>
-  <si>
-    <t>yjhW</t>
-  </si>
-  <si>
-    <t>mdaB/ygiN</t>
-  </si>
-  <si>
-    <t>yadK</t>
-  </si>
-  <si>
-    <t>tomB/acrB</t>
-  </si>
-  <si>
-    <t>ptsHI-crr terminator</t>
-  </si>
-  <si>
-    <t>pdxK</t>
-  </si>
-  <si>
-    <t>crp</t>
-  </si>
-  <si>
-    <t>carAB terminator</t>
-  </si>
-  <si>
-    <t>casD/casC</t>
-  </si>
-  <si>
-    <t>uraA/upp</t>
-  </si>
-  <si>
-    <t>yjhU/yjhF</t>
-  </si>
-  <si>
     <t>dgcE</t>
   </si>
   <si>
@@ -510,52 +540,55 @@
     <t>rpsMKD-rpoA-rplQ</t>
   </si>
   <si>
+    <t>yhdN-zntR</t>
+  </si>
+  <si>
     <t>metY-rimP-nusA-infB-rbfA-truB-rpsO-pnp</t>
   </si>
   <si>
+    <t>opgGH</t>
+  </si>
+  <si>
     <t>yceK</t>
   </si>
   <si>
-    <t>opgGH</t>
-  </si>
-  <si>
-    <t>yhdN-zntR</t>
-  </si>
-  <si>
     <t>metBL</t>
   </si>
   <si>
     <t>gntRKU</t>
   </si>
   <si>
+    <t>upp-uraA</t>
+  </si>
+  <si>
+    <t>gspCDEFGHIJKLMO</t>
+  </si>
+  <si>
+    <t>insH-4</t>
+  </si>
+  <si>
+    <t>glgS</t>
+  </si>
+  <si>
+    <t>epd-pgk-fbaA</t>
+  </si>
+  <si>
     <t>rrsB-gltT-rrlB-rrfB</t>
   </si>
   <si>
+    <t>ptsA-fsaB-gldA</t>
+  </si>
+  <si>
+    <t>yfdX-frc-oxc-yfdVE</t>
+  </si>
+  <si>
+    <t>tyrB</t>
+  </si>
+  <si>
     <t>fhuACDB</t>
   </si>
   <si>
-    <t>tyrB</t>
-  </si>
-  <si>
-    <t>yfdX-frc-oxc-yfdVE</t>
-  </si>
-  <si>
-    <t>ptsA-fsaB-gldA</t>
-  </si>
-  <si>
-    <t>epd-pgk-fbaA</t>
-  </si>
-  <si>
-    <t>insH-4</t>
-  </si>
-  <si>
-    <t>glgS</t>
-  </si>
-  <si>
-    <t>gspCDEFGHIJKLMO</t>
-  </si>
-  <si>
-    <t>upp-uraA</t>
+    <t>yjeF-tsaE-amiB-mutL-miaA-hfq-hflXKC</t>
   </si>
   <si>
     <t>yafDE</t>
@@ -564,30 +597,39 @@
     <t>casABCDE12</t>
   </si>
   <si>
+    <t>uidABC</t>
+  </si>
+  <si>
+    <t>yahIJ</t>
+  </si>
+  <si>
+    <t>moaABCDE</t>
+  </si>
+  <si>
+    <t>ymfH-xisE-intE</t>
+  </si>
+  <si>
+    <t>ynfEFGH-dmsD</t>
+  </si>
+  <si>
+    <t>flhDC</t>
+  </si>
+  <si>
     <t>napFDAGHBC-ccmABCDEFGH</t>
   </si>
   <si>
-    <t>uidABC</t>
-  </si>
-  <si>
-    <t>moaABCDE</t>
-  </si>
-  <si>
-    <t>ynfEFGH-dmsD</t>
-  </si>
-  <si>
-    <t>flhDC</t>
+    <t>carAB</t>
   </si>
   <si>
     <t>menFDHBCE</t>
   </si>
   <si>
-    <t>carAB</t>
-  </si>
-  <si>
     <t>ypfJ-tmcA</t>
   </si>
   <si>
+    <t>mutY-yggX-mltC-nupG</t>
+  </si>
+  <si>
     <t>atpIBEFHAGDC</t>
   </si>
   <si>
@@ -639,21 +681,21 @@
     <t>FNR</t>
   </si>
   <si>
+    <t>ArgR</t>
+  </si>
+  <si>
     <t>Fur</t>
   </si>
   <si>
-    <t>ArgR</t>
-  </si>
-  <si>
     <t>NarL</t>
   </si>
   <si>
+    <t>Lrp</t>
+  </si>
+  <si>
     <t>IHF</t>
   </si>
   <si>
-    <t>Lrp</t>
-  </si>
-  <si>
     <t>SlyA</t>
   </si>
   <si>
@@ -669,91 +711,91 @@
     <t>HypT</t>
   </si>
   <si>
+    <t>IscR</t>
+  </si>
+  <si>
+    <t>PepA</t>
+  </si>
+  <si>
+    <t>EvgA</t>
+  </si>
+  <si>
+    <t>PurR</t>
+  </si>
+  <si>
+    <t>RutR</t>
+  </si>
+  <si>
+    <t>TyrR</t>
+  </si>
+  <si>
+    <t>IdnR</t>
+  </si>
+  <si>
+    <t>PdhR</t>
+  </si>
+  <si>
+    <t>CpxR</t>
+  </si>
+  <si>
+    <t>BasR</t>
+  </si>
+  <si>
+    <t>AidB</t>
+  </si>
+  <si>
+    <t>Ada</t>
+  </si>
+  <si>
+    <t>OmpR</t>
+  </si>
+  <si>
     <t>FlhDC</t>
   </si>
   <si>
-    <t>EvgA</t>
-  </si>
-  <si>
-    <t>PurR</t>
-  </si>
-  <si>
-    <t>RutR</t>
-  </si>
-  <si>
-    <t>TyrR</t>
-  </si>
-  <si>
-    <t>PepA</t>
+    <t>NarP</t>
+  </si>
+  <si>
+    <t>CytR</t>
+  </si>
+  <si>
+    <t>NsrR</t>
+  </si>
+  <si>
+    <t>MatA</t>
+  </si>
+  <si>
+    <t>LrhA</t>
+  </si>
+  <si>
+    <t>RcsAB</t>
+  </si>
+  <si>
+    <t>FliZ</t>
+  </si>
+  <si>
+    <t>YjjQ</t>
+  </si>
+  <si>
+    <t>HdfR</t>
+  </si>
+  <si>
+    <t>QseB</t>
+  </si>
+  <si>
+    <t>AcrR</t>
+  </si>
+  <si>
+    <t>CueR</t>
+  </si>
+  <si>
+    <t>UidR</t>
+  </si>
+  <si>
+    <t>UxuR</t>
   </si>
   <si>
     <t>GntR</t>
-  </si>
-  <si>
-    <t>BasR</t>
-  </si>
-  <si>
-    <t>CpxR</t>
-  </si>
-  <si>
-    <t>PdhR</t>
-  </si>
-  <si>
-    <t>AidB</t>
-  </si>
-  <si>
-    <t>Ada</t>
-  </si>
-  <si>
-    <t>HdfR</t>
-  </si>
-  <si>
-    <t>IscR</t>
-  </si>
-  <si>
-    <t>NarP</t>
-  </si>
-  <si>
-    <t>NsrR</t>
-  </si>
-  <si>
-    <t>CytR</t>
-  </si>
-  <si>
-    <t>YjjQ</t>
-  </si>
-  <si>
-    <t>QseB</t>
-  </si>
-  <si>
-    <t>FliZ</t>
-  </si>
-  <si>
-    <t>LrhA</t>
-  </si>
-  <si>
-    <t>OmpR</t>
-  </si>
-  <si>
-    <t>MatA</t>
-  </si>
-  <si>
-    <t>RcsAB</t>
-  </si>
-  <si>
-    <t>AcrR</t>
-  </si>
-  <si>
-    <t>CueR</t>
-  </si>
-  <si>
-    <t>UxuR</t>
-  </si>
-  <si>
-    <t>UidR</t>
-  </si>
-  <si>
-    <t>IdnR</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1153,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1133,7 +1175,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -1144,7 +1186,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C3">
         <v>21</v>
@@ -1155,7 +1197,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -1166,7 +1208,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -1177,7 +1219,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1188,7 +1230,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -1199,7 +1241,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -1210,7 +1252,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -1221,7 +1263,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1232,7 +1274,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1243,7 +1285,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1254,7 +1296,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1265,7 +1307,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1276,7 +1318,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1287,7 +1329,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1298,7 +1340,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1309,7 +1351,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1320,7 +1362,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1331,7 +1373,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1342,7 +1384,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1353,7 +1395,7 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1364,7 +1406,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1375,7 +1417,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1386,7 +1428,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1397,7 +1439,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1408,7 +1450,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1419,7 +1461,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1430,7 +1472,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1441,7 +1483,7 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1452,7 +1494,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1463,7 +1505,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1474,7 +1516,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1485,7 +1527,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -1496,7 +1538,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1507,7 +1549,7 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1518,7 +1560,7 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1529,7 +1571,7 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1540,7 +1582,7 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1551,7 +1593,7 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1562,7 +1604,7 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1573,7 +1615,7 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -1584,7 +1626,7 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1595,7 +1637,7 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -1606,7 +1648,7 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -1617,7 +1659,7 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1628,7 +1670,7 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1639,7 +1681,7 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -1650,7 +1692,7 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -1661,7 +1703,7 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -1672,7 +1714,7 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -1683,7 +1725,7 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -1694,7 +1736,7 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -1705,7 +1747,7 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1716,7 +1758,7 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1727,7 +1769,7 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -1738,7 +1780,7 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -1749,7 +1791,7 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -1760,7 +1802,7 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -1771,7 +1813,7 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -1782,7 +1824,7 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -1793,7 +1835,7 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -1804,7 +1846,7 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -1815,7 +1857,7 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -1826,7 +1868,7 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -1837,7 +1879,7 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -1848,7 +1890,7 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -1859,7 +1901,7 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -1870,7 +1912,7 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -1881,7 +1923,7 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -1892,7 +1934,7 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -1903,7 +1945,7 @@
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -1914,7 +1956,7 @@
         <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -1925,7 +1967,7 @@
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -1936,7 +1978,7 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -1947,7 +1989,7 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -1958,7 +2000,7 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -1969,9 +2011,64 @@
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" t="s">
+        <v>161</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" t="s">
+        <v>162</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81" t="s">
+        <v>163</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" t="s">
+        <v>164</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83" t="s">
+        <v>165</v>
+      </c>
+      <c r="C83">
         <v>1</v>
       </c>
     </row>
@@ -1982,7 +2079,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1990,7 +2087,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1998,7 +2095,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="B2">
         <v>32</v>
@@ -2006,7 +2103,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B3">
         <v>21</v>
@@ -2014,7 +2111,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="B4">
         <v>11</v>
@@ -2022,7 +2119,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B5">
         <v>9</v>
@@ -2030,7 +2127,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -2038,7 +2135,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -2046,7 +2143,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -2054,7 +2151,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -2062,7 +2159,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -2070,7 +2167,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -2078,7 +2175,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>96</v>
+        <v>175</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -2086,7 +2183,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>165</v>
+        <v>100</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -2094,7 +2191,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -2102,7 +2199,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -2110,7 +2207,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>95</v>
+        <v>178</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -2118,7 +2215,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>168</v>
+        <v>101</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -2126,7 +2223,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2134,7 +2231,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>170</v>
+        <v>112</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2142,7 +2239,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>118</v>
+        <v>180</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -2150,7 +2247,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>119</v>
+        <v>181</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2158,7 +2255,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2166,7 +2263,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2174,7 +2271,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>173</v>
+        <v>118</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2182,7 +2279,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2190,7 +2287,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2198,7 +2295,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2206,7 +2303,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2214,7 +2311,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2222,7 +2319,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -2230,7 +2327,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2238,7 +2335,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -2246,7 +2343,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -2254,7 +2351,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -2262,7 +2359,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -2270,7 +2367,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>128</v>
+        <v>192</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -2278,7 +2375,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>184</v>
+        <v>136</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -2286,7 +2383,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2294,7 +2391,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2302,7 +2399,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>186</v>
+        <v>146</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2310,7 +2407,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>134</v>
+        <v>195</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -2318,7 +2415,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>135</v>
+        <v>196</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -2326,7 +2423,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>137</v>
+        <v>197</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2334,7 +2431,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>187</v>
+        <v>141</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -2342,7 +2439,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2350,7 +2447,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2358,7 +2455,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>190</v>
+        <v>138</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2366,7 +2463,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2374,7 +2471,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>143</v>
+        <v>200</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -2382,7 +2479,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2390,7 +2487,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -2398,7 +2495,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -2406,7 +2503,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>149</v>
+        <v>204</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -2414,7 +2511,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>150</v>
+        <v>205</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -2422,9 +2519,49 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B60">
         <v>1</v>
       </c>
     </row>
@@ -2443,7 +2580,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2451,7 +2588,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="B2">
         <v>74</v>
@@ -2459,7 +2596,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="B3">
         <v>32</v>
@@ -2467,7 +2604,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="B4">
         <v>13</v>
@@ -2475,7 +2612,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="B5">
         <v>11</v>
@@ -2483,7 +2620,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="B6">
         <v>11</v>
@@ -2491,7 +2628,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="B7">
         <v>11</v>
@@ -2499,7 +2636,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -2507,7 +2644,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -2515,7 +2652,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -2523,7 +2660,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -2531,7 +2668,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -2539,7 +2676,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -2547,7 +2684,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -2555,7 +2692,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -2563,7 +2700,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -2571,7 +2708,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -2579,7 +2716,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -2587,7 +2724,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -2595,7 +2732,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -2603,7 +2740,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -2611,7 +2748,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -2619,7 +2756,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2627,7 +2764,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2635,7 +2772,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2643,7 +2780,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2651,7 +2788,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2659,7 +2796,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2667,7 +2804,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2675,7 +2812,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -2683,7 +2820,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2691,7 +2828,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -2699,7 +2836,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -2707,7 +2844,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -2715,7 +2852,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -2723,7 +2860,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -2731,7 +2868,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -2739,7 +2876,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2747,7 +2884,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2755,7 +2892,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2763,7 +2900,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -2771,7 +2908,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -2779,7 +2916,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2787,7 +2924,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -2795,7 +2932,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2803,7 +2940,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2811,7 +2948,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2819,7 +2956,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2827,7 +2964,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -2835,7 +2972,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2843,7 +2980,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="B51">
         <v>1</v>

</xml_diff>